<commit_message>
Working on expression sheet parsing/testing
</commit_message>
<xml_diff>
--- a/test-files/expression-data-test-sheets/expression_sheet_empty_row.xlsx
+++ b/test-files/expression-data-test-sheets/expression_sheet_empty_row.xlsx
@@ -8,18 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\GRNsight\test-files\expression-data-test-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F05EE0-8823-442D-9D90-C41D443BA42C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B9AD6F-9773-4C86-9FCC-8E29F3D60041}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="production_rates" sheetId="5" r:id="rId1"/>
-    <sheet name="degradation_rates" sheetId="4" r:id="rId2"/>
-    <sheet name="wt_log2_expression" sheetId="6" r:id="rId3"/>
-    <sheet name="network" sheetId="2" r:id="rId4"/>
-    <sheet name="network_weights" sheetId="3" r:id="rId5"/>
-    <sheet name="optimization_parameters" sheetId="9" r:id="rId6"/>
-    <sheet name="threshold_b" sheetId="10" r:id="rId7"/>
+    <sheet name="wt_log2_expression" sheetId="6" r:id="rId1"/>
+    <sheet name="network" sheetId="2" r:id="rId2"/>
+    <sheet name="network_weights" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>ACE2</t>
   </si>
@@ -47,83 +43,11 @@
   <si>
     <t>id</t>
   </si>
-  <si>
-    <t>degradation_rate</t>
-  </si>
-  <si>
-    <t>production_rate</t>
-  </si>
-  <si>
-    <t>threshold_b</t>
-  </si>
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>kk_max</t>
-  </si>
-  <si>
-    <t>MaxIter</t>
-  </si>
-  <si>
-    <t>TolFun</t>
-  </si>
-  <si>
-    <t>MaxFunEval</t>
-  </si>
-  <si>
-    <t>TolX</t>
-  </si>
-  <si>
-    <t>production_function</t>
-  </si>
-  <si>
-    <t>L_curve</t>
-  </si>
-  <si>
-    <t>estimate_params</t>
-  </si>
-  <si>
-    <t>make_graphs</t>
-  </si>
-  <si>
-    <t>fix_P</t>
-  </si>
-  <si>
-    <t>fix_b</t>
-  </si>
-  <si>
-    <t>expression_timepoints</t>
-  </si>
-  <si>
-    <t>Strain</t>
-  </si>
-  <si>
-    <t>simulation_timepoints</t>
-  </si>
-  <si>
-    <t>Sigmoid</t>
-  </si>
-  <si>
-    <t>wt</t>
-  </si>
-  <si>
-    <t>optimization_parameter</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>dgln3</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -532,12 +456,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="348">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1223,68 +1145,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="2"/>
+    <col min="1" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.22359999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.43319999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.2009</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1297,54 +1279,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="2"/>
+    <col min="1" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>0.1118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>0.21659999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.10050000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1358,220 +1359,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1649,231 +1436,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>